<commit_message>
RDM-5519: Improvising the test case. We are uploading the definition, as well as matching all of the CaseType attributes in same test case.
</commit_message>
<xml_diff>
--- a/aat/src/resource/CCD_CNP_27_Missing_CaseType_ACL_Info.xlsx
+++ b/aat/src/resource/CCD_CNP_27_Missing_CaseType_ACL_Info.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1080" windowWidth="29180" windowHeight="16620" tabRatio="823" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="1080" windowWidth="29177" windowHeight="16620" tabRatio="823" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1876" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1878" uniqueCount="280">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -891,6 +891,15 @@
   <si>
     <t>C - Create, R - Read, U - Update, D - Delete
 MustBe1OrManyOf: &lt;C,R,U,D&gt; MaxLength: 5</t>
+  </si>
+  <si>
+    <t>AAT1</t>
+  </si>
+  <si>
+    <t>Demo case</t>
+  </si>
+  <si>
+    <t>Demonstrate everyhting CCD can do!</t>
   </si>
 </sst>
 </file>
@@ -1759,16 +1768,16 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.3828125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.1796875" customWidth="1"/>
-    <col min="5" max="5" width="43.81640625" customWidth="1"/>
+    <col min="1" max="1" width="17.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.3828125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.3828125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.15234375" customWidth="1"/>
+    <col min="5" max="5" width="43.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1783,7 +1792,7 @@
       </c>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6" t="s">
@@ -1813,7 +1822,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>42736</v>
       </c>
@@ -1855,17 +1864,17 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.3828125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.1796875" customWidth="1"/>
-    <col min="5" max="5" width="19.36328125" customWidth="1"/>
-    <col min="6" max="6" width="12.6328125" customWidth="1"/>
+    <col min="1" max="1" width="27.3828125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.3828125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.84375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.15234375" customWidth="1"/>
+    <col min="5" max="5" width="19.3828125" customWidth="1"/>
+    <col min="6" max="6" width="12.61328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -1881,7 +1890,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" s="30" customFormat="1" ht="39" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="30" customFormat="1" ht="38.6" x14ac:dyDescent="0.35">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="31" t="s">
@@ -1897,7 +1906,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="14.6" x14ac:dyDescent="0.4">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -1917,7 +1926,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="14.6" x14ac:dyDescent="0.4">
       <c r="A4" s="23">
         <v>42736</v>
       </c>
@@ -1935,7 +1944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="14" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" s="14" customFormat="1" ht="14.6" x14ac:dyDescent="0.4">
       <c r="A5" s="23">
         <v>42736</v>
       </c>
@@ -1953,7 +1962,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="14" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" s="14" customFormat="1" ht="14.6" x14ac:dyDescent="0.4">
       <c r="A6" s="23">
         <v>42736</v>
       </c>
@@ -1971,7 +1980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="14" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" s="14" customFormat="1" ht="14.6" x14ac:dyDescent="0.4">
       <c r="A7" s="23">
         <v>42736</v>
       </c>
@@ -2029,18 +2038,18 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.81640625" style="70" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" style="71" customWidth="1"/>
-    <col min="3" max="3" width="29.81640625" style="71" customWidth="1"/>
-    <col min="4" max="4" width="19.81640625" style="71" customWidth="1"/>
-    <col min="5" max="5" width="20.1796875" style="71" customWidth="1"/>
-    <col min="6" max="6" width="15.36328125" style="71" customWidth="1"/>
-    <col min="7" max="16384" width="8.81640625" style="14"/>
+    <col min="1" max="1" width="28.84375" style="70" customWidth="1"/>
+    <col min="2" max="2" width="15.4609375" style="71" customWidth="1"/>
+    <col min="3" max="3" width="29.84375" style="71" customWidth="1"/>
+    <col min="4" max="4" width="19.84375" style="71" customWidth="1"/>
+    <col min="5" max="5" width="20.15234375" style="71" customWidth="1"/>
+    <col min="6" max="6" width="15.3828125" style="71" customWidth="1"/>
+    <col min="7" max="16384" width="8.84375" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" ht="18.45" x14ac:dyDescent="0.5">
       <c r="A1" s="62" t="s">
         <v>130</v>
       </c>
@@ -2056,7 +2065,7 @@
       <c r="E1" s="66"/>
       <c r="F1" s="66"/>
     </row>
-    <row r="2" spans="1:6" ht="43.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="43.75" x14ac:dyDescent="0.3">
       <c r="A2" s="67"/>
       <c r="B2" s="67"/>
       <c r="C2" s="68" t="s">
@@ -2072,7 +2081,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="69" t="s">
         <v>8</v>
       </c>
@@ -2092,7 +2101,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="13">
         <v>42736</v>
       </c>
@@ -2110,7 +2119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="13">
         <v>42736</v>
       </c>
@@ -2168,14 +2177,14 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.3828125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.36328125" customWidth="1"/>
-    <col min="4" max="4" width="16.36328125" customWidth="1"/>
-    <col min="5" max="5" width="19.36328125" customWidth="1"/>
-    <col min="6" max="6" width="12.6328125" customWidth="1"/>
+    <col min="1" max="1" width="34.3828125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.3828125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.3828125" customWidth="1"/>
+    <col min="4" max="4" width="16.3828125" customWidth="1"/>
+    <col min="5" max="5" width="19.3828125" customWidth="1"/>
+    <col min="6" max="6" width="12.61328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -2194,7 +2203,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" s="30" customFormat="1" ht="52" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="30" customFormat="1" ht="51.45" x14ac:dyDescent="0.35">
       <c r="A2" s="34"/>
       <c r="B2" s="34"/>
       <c r="C2" s="31" t="s">
@@ -2210,7 +2219,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="14.6" x14ac:dyDescent="0.4">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -2230,7 +2239,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="14.6" x14ac:dyDescent="0.4">
       <c r="A4" s="23">
         <v>42736</v>
       </c>
@@ -2248,7 +2257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="14.6" x14ac:dyDescent="0.4">
       <c r="A5" s="23">
         <v>42736</v>
       </c>
@@ -2266,7 +2275,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="14" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" s="14" customFormat="1" ht="14.6" x14ac:dyDescent="0.4">
       <c r="A6" s="23">
         <v>42736</v>
       </c>
@@ -2284,7 +2293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="14" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" s="14" customFormat="1" ht="14.6" x14ac:dyDescent="0.4">
       <c r="A7" s="23">
         <v>42736</v>
       </c>
@@ -2342,19 +2351,19 @@
       <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.3828125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="8.81640625" customWidth="1"/>
-    <col min="3" max="3" width="27.81640625" customWidth="1"/>
-    <col min="4" max="4" width="31.6328125" customWidth="1"/>
+    <col min="2" max="2" width="8.84375" customWidth="1"/>
+    <col min="3" max="3" width="27.84375" customWidth="1"/>
+    <col min="4" max="4" width="31.61328125" customWidth="1"/>
     <col min="5" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="16.36328125" customWidth="1"/>
-    <col min="8" max="8" width="40.81640625" customWidth="1"/>
+    <col min="7" max="7" width="16.3828125" customWidth="1"/>
+    <col min="8" max="8" width="40.84375" customWidth="1"/>
     <col min="9" max="9" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>48</v>
       </c>
@@ -2373,7 +2382,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="34"/>
       <c r="B2" s="34"/>
       <c r="C2" s="31" t="s">
@@ -2427,7 +2436,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="25">
         <v>42736</v>
       </c>
@@ -2454,7 +2463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="27">
         <v>42736</v>
       </c>
@@ -2481,7 +2490,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="27">
         <v>42736</v>
       </c>
@@ -2508,7 +2517,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="27">
         <v>42736</v>
       </c>
@@ -2535,7 +2544,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="27">
         <v>42736</v>
       </c>
@@ -2562,7 +2571,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="27">
         <v>42736</v>
       </c>
@@ -2589,7 +2598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="27">
         <v>42736</v>
       </c>
@@ -2616,7 +2625,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="27">
         <v>42736</v>
       </c>
@@ -2643,7 +2652,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="27">
         <v>42736</v>
       </c>
@@ -2670,7 +2679,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="27">
         <v>42736</v>
       </c>
@@ -2697,7 +2706,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="27">
         <v>42736</v>
       </c>
@@ -2724,7 +2733,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="27">
         <v>42736</v>
       </c>
@@ -2751,7 +2760,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="27">
         <v>42736</v>
       </c>
@@ -2778,7 +2787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="27">
         <v>42736</v>
       </c>
@@ -2805,7 +2814,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="27">
         <v>42736</v>
       </c>
@@ -2832,7 +2841,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="27">
         <v>42736</v>
       </c>
@@ -2859,7 +2868,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="27">
         <v>42736</v>
       </c>
@@ -2886,7 +2895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="27">
         <v>42736</v>
       </c>
@@ -2913,7 +2922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="27">
         <v>42736</v>
       </c>
@@ -2940,7 +2949,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="27">
         <v>42736</v>
       </c>
@@ -2967,7 +2976,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="27">
         <v>42736</v>
       </c>
@@ -2994,7 +3003,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="27">
         <v>42736</v>
       </c>
@@ -3021,7 +3030,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="27">
         <v>42736</v>
       </c>
@@ -3048,7 +3057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="27">
         <v>42736</v>
       </c>
@@ -3075,7 +3084,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="27">
         <v>42736</v>
       </c>
@@ -3102,7 +3111,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="27">
         <v>42736</v>
       </c>
@@ -3129,7 +3138,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="27">
         <v>42736</v>
       </c>
@@ -3156,7 +3165,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="27">
         <v>42736</v>
       </c>
@@ -3183,7 +3192,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="27">
         <v>42736</v>
       </c>
@@ -3210,7 +3219,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="27">
         <v>42736</v>
       </c>
@@ -3237,7 +3246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="27">
         <v>42736</v>
       </c>
@@ -3264,7 +3273,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A35" s="27">
         <v>42736</v>
       </c>
@@ -3291,7 +3300,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="27">
         <v>42736</v>
       </c>
@@ -3348,14 +3357,14 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.36328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.3828125" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.1796875" customWidth="1"/>
-    <col min="2" max="2" width="17.81640625" customWidth="1"/>
-    <col min="3" max="3" width="18.36328125" customWidth="1"/>
-    <col min="4" max="4" width="28.36328125" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.81640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.15234375" customWidth="1"/>
+    <col min="2" max="2" width="17.84375" customWidth="1"/>
+    <col min="3" max="3" width="18.3828125" customWidth="1"/>
+    <col min="4" max="4" width="28.3828125" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.84375" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.84375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="14" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -3373,7 +3382,7 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="3" spans="1:6" s="38" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" s="38" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="37" t="s">
         <v>8</v>
       </c>
@@ -3393,7 +3402,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="72">
         <v>42736</v>
       </c>
@@ -3432,15 +3441,15 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.3828125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.36328125" customWidth="1"/>
-    <col min="3" max="3" width="27.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.81640625" customWidth="1"/>
+    <col min="1" max="1" width="33.3828125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.3828125" customWidth="1"/>
+    <col min="3" max="3" width="27.3828125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
@@ -3455,7 +3464,7 @@
       </c>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" s="30" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="30" customFormat="1" ht="64.3" x14ac:dyDescent="0.35">
       <c r="A2" s="34"/>
       <c r="B2" s="34"/>
       <c r="C2" s="31" t="s">
@@ -3468,7 +3477,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
@@ -3485,7 +3494,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A4" s="29">
         <v>42736</v>
       </c>
@@ -3500,7 +3509,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="14" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="14" customFormat="1" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A5" s="29">
         <v>42736</v>
       </c>
@@ -3534,15 +3543,15 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.1796875" style="61" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" style="61" customWidth="1"/>
-    <col min="3" max="3" width="27.81640625" style="61" customWidth="1"/>
-    <col min="4" max="4" width="18.6328125" style="61" customWidth="1"/>
+    <col min="1" max="1" width="28.15234375" style="61" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.4609375" style="61" customWidth="1"/>
+    <col min="3" max="3" width="27.84375" style="61" customWidth="1"/>
+    <col min="4" max="4" width="18.61328125" style="61" customWidth="1"/>
     <col min="5" max="5" width="27" style="61" customWidth="1"/>
-    <col min="6" max="6" width="14.453125" style="61" customWidth="1"/>
-    <col min="7" max="16384" width="8.81640625" style="54"/>
+    <col min="6" max="6" width="14.4609375" style="61" customWidth="1"/>
+    <col min="7" max="16384" width="8.84375" style="54"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.4">
@@ -3561,7 +3570,7 @@
       <c r="E1" s="53"/>
       <c r="F1" s="53"/>
     </row>
-    <row r="2" spans="1:6" ht="65" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="64.3" x14ac:dyDescent="0.35">
       <c r="A2" s="55"/>
       <c r="B2" s="55"/>
       <c r="C2" s="56" t="s">
@@ -3597,7 +3606,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="59">
         <v>42736</v>
       </c>
@@ -3615,7 +3624,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="59">
         <v>42736</v>
       </c>
@@ -3633,7 +3642,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="59">
         <v>42736</v>
       </c>
@@ -3651,7 +3660,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="59">
         <v>42736</v>
       </c>
@@ -3669,7 +3678,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="59">
         <v>42736</v>
       </c>
@@ -3687,7 +3696,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="59">
         <v>42736</v>
       </c>
@@ -3724,16 +3733,16 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.3828125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.81640625" customWidth="1"/>
+    <col min="1" max="1" width="34.3828125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.3828125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.84375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.61328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>61</v>
       </c>
@@ -3749,7 +3758,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" s="30" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="30" customFormat="1" ht="64.3" x14ac:dyDescent="0.35">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="31" t="s">
@@ -3765,7 +3774,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="33" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" s="33" customFormat="1" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
@@ -3785,7 +3794,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="72">
         <v>42736</v>
       </c>
@@ -3802,7 +3811,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="72">
         <v>42736</v>
       </c>
@@ -3819,7 +3828,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="72">
         <v>42736</v>
       </c>
@@ -3836,7 +3845,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="72">
         <v>42736</v>
       </c>
@@ -3853,7 +3862,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="72">
         <v>42736</v>
       </c>
@@ -3870,7 +3879,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="72">
         <v>42736</v>
       </c>
@@ -3887,7 +3896,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="72">
         <v>42736</v>
       </c>
@@ -3904,7 +3913,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="72">
         <v>42736</v>
       </c>
@@ -3921,7 +3930,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="72">
         <v>42736</v>
       </c>
@@ -3938,7 +3947,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="72">
         <v>42736</v>
       </c>
@@ -3955,7 +3964,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="72">
         <v>42736</v>
       </c>
@@ -3972,7 +3981,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="72">
         <v>42736</v>
       </c>
@@ -4008,16 +4017,16 @@
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.3828125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.81640625" customWidth="1"/>
+    <col min="2" max="2" width="15.3828125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.3828125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.3828125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>60</v>
       </c>
@@ -4032,7 +4041,7 @@
       </c>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:6" ht="78" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="64.3" x14ac:dyDescent="0.35">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6" t="s">
@@ -4048,7 +4057,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="33" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" s="33" customFormat="1" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
@@ -4068,7 +4077,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="72">
         <v>42736</v>
       </c>
@@ -4085,7 +4094,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="72">
         <v>42736</v>
       </c>
@@ -4102,7 +4111,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="72">
         <v>42736</v>
       </c>
@@ -4119,7 +4128,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="72">
         <v>42736</v>
       </c>
@@ -4136,7 +4145,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="72">
         <v>42736</v>
       </c>
@@ -4153,7 +4162,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="72">
         <v>42736</v>
       </c>
@@ -4170,7 +4179,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="72">
         <v>42736</v>
       </c>
@@ -4187,7 +4196,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="72">
         <v>42736</v>
       </c>
@@ -4204,7 +4213,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="72">
         <v>42736</v>
       </c>
@@ -4221,7 +4230,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="72">
         <v>42736</v>
       </c>
@@ -4238,7 +4247,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="72">
         <v>42736</v>
       </c>
@@ -4255,7 +4264,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="72">
         <v>42736</v>
       </c>
@@ -4272,7 +4281,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="72">
         <v>42736</v>
       </c>
@@ -4290,7 +4299,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="72">
         <v>42736</v>
       </c>
@@ -4307,7 +4316,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="72">
         <v>42736</v>
       </c>
@@ -4325,7 +4334,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="72">
         <v>42736</v>
       </c>
@@ -4342,7 +4351,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="72">
         <v>42736</v>
       </c>
@@ -4359,7 +4368,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="72">
         <v>42736</v>
       </c>
@@ -4376,7 +4385,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="72">
         <v>42736</v>
       </c>
@@ -4393,7 +4402,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="72">
         <v>42736</v>
       </c>
@@ -4410,7 +4419,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="72">
         <v>42736</v>
       </c>
@@ -4427,7 +4436,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="72">
         <v>42736</v>
       </c>
@@ -4444,7 +4453,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="72">
         <v>42736</v>
       </c>
@@ -4461,7 +4470,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="72">
         <v>42736</v>
       </c>
@@ -4478,7 +4487,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="72">
         <v>42736</v>
       </c>
@@ -4495,7 +4504,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="72">
         <v>42736</v>
       </c>
@@ -4512,7 +4521,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="72">
         <v>42736</v>
       </c>
@@ -4529,7 +4538,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="72">
         <v>42736</v>
       </c>
@@ -4546,7 +4555,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="72">
         <v>42736</v>
       </c>
@@ -4563,7 +4572,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="72">
         <v>42736</v>
       </c>
@@ -4580,7 +4589,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="72">
         <v>42736</v>
       </c>
@@ -4597,7 +4606,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="72">
         <v>42736</v>
       </c>
@@ -4614,7 +4623,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="72">
         <v>42736</v>
       </c>
@@ -4650,19 +4659,19 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.1796875" style="81" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.453125" style="81" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.453125" style="81" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.36328125" style="81" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="57.6328125" style="81" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.36328125" style="81" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.36328125" style="81" customWidth="1"/>
-    <col min="8" max="16384" width="10.81640625" style="81"/>
+    <col min="1" max="1" width="33.15234375" style="81" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.4609375" style="81" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.4609375" style="81" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.3828125" style="81" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.61328125" style="81" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.3828125" style="81" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.3828125" style="81" customWidth="1"/>
+    <col min="8" max="16384" width="10.84375" style="81"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A1" s="76" t="s">
         <v>271</v>
       </c>
@@ -4679,7 +4688,7 @@
       <c r="F1" s="80"/>
       <c r="G1" s="80"/>
     </row>
-    <row r="2" spans="1:7" ht="65" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="64.3" x14ac:dyDescent="0.35">
       <c r="A2" s="82"/>
       <c r="B2" s="82"/>
       <c r="C2" s="83" t="s">
@@ -4698,7 +4707,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="84" t="s">
         <v>8</v>
       </c>
@@ -4721,7 +4730,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="72">
         <v>42736</v>
       </c>
@@ -4741,7 +4750,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="72">
         <v>42736</v>
       </c>
@@ -4761,7 +4770,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="72">
         <v>42736</v>
       </c>
@@ -4791,24 +4800,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:I5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.3828125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.84375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.81640625" customWidth="1"/>
-    <col min="5" max="5" width="15.81640625" customWidth="1"/>
-    <col min="6" max="6" width="16.36328125" customWidth="1"/>
-    <col min="7" max="7" width="20.81640625" customWidth="1"/>
-    <col min="8" max="8" width="16.36328125" customWidth="1"/>
+    <col min="3" max="3" width="27.84375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.84375" customWidth="1"/>
+    <col min="5" max="5" width="15.84375" customWidth="1"/>
+    <col min="6" max="6" width="16.3828125" customWidth="1"/>
+    <col min="7" max="7" width="20.84375" customWidth="1"/>
+    <col min="8" max="8" width="16.3828125" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -4827,7 +4836,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9" s="30" customFormat="1" ht="74" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="30" customFormat="1" ht="74.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="31" t="s">
@@ -4848,9 +4857,7 @@
       <c r="H2" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="I2" s="31" t="s">
-        <v>90</v>
-      </c>
+      <c r="I2" s="31"/>
     </row>
     <row r="3" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
@@ -4877,19 +4884,30 @@
       <c r="H3" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="I3" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
+      <c r="I3" s="8"/>
+    </row>
+    <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="13">
+        <v>42736</v>
+      </c>
       <c r="B4" s="13"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="28"/>
-    </row>
-    <row r="5" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="28" t="s">
+        <v>277</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>278</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>279</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>234</v>
+      </c>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+    </row>
+    <row r="5" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="28"/>
@@ -4924,22 +4942,22 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.3828125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.81640625" customWidth="1"/>
-    <col min="4" max="4" width="41.36328125" customWidth="1"/>
-    <col min="5" max="5" width="40.81640625" customWidth="1"/>
-    <col min="6" max="6" width="24.81640625" customWidth="1"/>
+    <col min="1" max="1" width="14.3828125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.3828125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.84375" customWidth="1"/>
+    <col min="4" max="4" width="41.3828125" customWidth="1"/>
+    <col min="5" max="5" width="40.84375" customWidth="1"/>
+    <col min="6" max="6" width="24.84375" customWidth="1"/>
     <col min="7" max="8" width="37" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="20.36328125" customWidth="1"/>
+    <col min="10" max="10" width="20.3828125" customWidth="1"/>
     <col min="11" max="11" width="20" customWidth="1"/>
-    <col min="12" max="13" width="8.81640625" customWidth="1"/>
+    <col min="12" max="13" width="8.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -4959,7 +4977,7 @@
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:13" s="30" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="30" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="31" t="s">
@@ -5033,7 +5051,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>42736</v>
       </c>
@@ -5062,7 +5080,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>42736</v>
       </c>
@@ -5091,7 +5109,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>42736</v>
       </c>
@@ -5120,7 +5138,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>42736</v>
       </c>
@@ -5149,7 +5167,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>42736</v>
       </c>
@@ -5178,7 +5196,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>42736</v>
       </c>
@@ -5207,7 +5225,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>42736</v>
       </c>
@@ -5236,7 +5254,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <v>42736</v>
       </c>
@@ -5265,7 +5283,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>42736</v>
       </c>
@@ -5294,7 +5312,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>42736</v>
       </c>
@@ -5325,7 +5343,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="13">
         <v>42736</v>
       </c>
@@ -5356,7 +5374,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="13">
         <v>42736</v>
       </c>
@@ -5387,7 +5405,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="13">
         <v>42736</v>
       </c>
@@ -5416,7 +5434,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13">
         <v>42736</v>
       </c>
@@ -5445,7 +5463,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="13">
         <v>42736</v>
       </c>
@@ -5474,7 +5492,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13">
         <v>42736</v>
       </c>
@@ -5505,7 +5523,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13">
         <v>42736</v>
       </c>
@@ -5534,7 +5552,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13">
         <v>42736</v>
       </c>
@@ -5563,7 +5581,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13">
         <v>42736</v>
       </c>
@@ -5592,7 +5610,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13">
         <v>42736</v>
       </c>
@@ -5621,7 +5639,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="13">
         <v>42736</v>
       </c>
@@ -5650,7 +5668,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="13">
         <v>42736</v>
       </c>
@@ -5679,7 +5697,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="13">
         <v>42736</v>
       </c>
@@ -5708,7 +5726,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="13">
         <v>42736</v>
       </c>
@@ -5737,7 +5755,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="28" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="13">
         <v>42736</v>
       </c>
@@ -5766,7 +5784,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="13">
         <v>42736</v>
       </c>
@@ -5795,7 +5813,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="30" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="13">
         <v>42736</v>
       </c>
@@ -5826,7 +5844,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="31" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="13">
         <v>42736</v>
       </c>
@@ -5857,7 +5875,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="13">
         <v>42736</v>
       </c>
@@ -5888,7 +5906,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="33" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="13">
         <v>42736</v>
       </c>
@@ -5917,7 +5935,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="34" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="13">
         <v>42736</v>
       </c>
@@ -5946,7 +5964,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="13">
         <v>42736</v>
       </c>
@@ -5977,7 +5995,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="36" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="13">
         <v>42736</v>
       </c>
@@ -6033,15 +6051,15 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.3828125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="31.6328125" customWidth="1"/>
-    <col min="5" max="5" width="28.36328125" customWidth="1"/>
+    <col min="1" max="1" width="15.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.3828125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="31.61328125" customWidth="1"/>
+    <col min="5" max="5" width="28.3828125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -6056,7 +6074,7 @@
       </c>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="31" t="s">
@@ -6086,7 +6104,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15">
         <v>42736</v>
       </c>
@@ -6101,7 +6119,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15">
         <v>42736</v>
       </c>
@@ -6116,7 +6134,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15">
         <v>42736</v>
       </c>
@@ -6131,7 +6149,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15">
         <v>42736</v>
       </c>
@@ -6146,7 +6164,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15">
         <v>42736</v>
       </c>
@@ -6161,7 +6179,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15">
         <v>42736</v>
       </c>
@@ -6176,7 +6194,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="15">
         <v>42736</v>
       </c>
@@ -6191,7 +6209,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15">
         <v>42736</v>
       </c>
@@ -6206,7 +6224,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15">
         <v>42736</v>
       </c>
@@ -6221,7 +6239,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15">
         <v>42736</v>
       </c>
@@ -6236,7 +6254,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15">
         <v>42736</v>
       </c>
@@ -6278,24 +6296,24 @@
       <selection activeCell="D6" sqref="D6:D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.3828125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.36328125" customWidth="1"/>
-    <col min="6" max="6" width="18.6328125" customWidth="1"/>
+    <col min="1" max="1" width="21.61328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.3828125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.3828125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.3828125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.3828125" customWidth="1"/>
+    <col min="6" max="6" width="18.61328125" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="24.81640625" customWidth="1"/>
-    <col min="9" max="9" width="24.81640625" style="14" customWidth="1"/>
+    <col min="8" max="8" width="24.84375" customWidth="1"/>
+    <col min="9" max="9" width="24.84375" style="14" customWidth="1"/>
     <col min="10" max="10" width="37" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
     <col min="12" max="12" width="20" customWidth="1"/>
-    <col min="13" max="14" width="8.81640625" customWidth="1"/>
+    <col min="13" max="14" width="8.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -6316,7 +6334,7 @@
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
     </row>
-    <row r="2" spans="1:14" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6" t="s">
@@ -6458,7 +6476,7 @@
       <c r="M5" s="35"/>
       <c r="N5" s="8"/>
     </row>
-    <row r="6" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11">
         <v>42736</v>
       </c>
@@ -6486,7 +6504,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>42736</v>
       </c>
@@ -6516,7 +6534,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>42736</v>
       </c>
@@ -6571,18 +6589,18 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.3828125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.36328125" customWidth="1"/>
-    <col min="2" max="2" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.36328125" customWidth="1"/>
-    <col min="5" max="5" width="31.6328125" customWidth="1"/>
+    <col min="1" max="1" width="11.3828125" customWidth="1"/>
+    <col min="2" max="2" width="15.3828125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.84375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.3828125" customWidth="1"/>
+    <col min="5" max="5" width="31.61328125" customWidth="1"/>
     <col min="6" max="6" width="32" customWidth="1"/>
-    <col min="7" max="7" width="12.6328125" customWidth="1"/>
+    <col min="7" max="7" width="12.61328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
@@ -6599,7 +6617,7 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" spans="1:7" ht="61" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="61" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -6635,7 +6653,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11">
         <v>42736</v>
       </c>
@@ -6654,7 +6672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>42736</v>
       </c>
@@ -6673,7 +6691,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>42736</v>
       </c>
@@ -6692,7 +6710,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>42736</v>
       </c>
@@ -6711,7 +6729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>42736</v>
       </c>
@@ -6730,7 +6748,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>42736</v>
       </c>
@@ -6779,28 +6797,28 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.3828125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.6328125" customWidth="1"/>
-    <col min="6" max="6" width="45.36328125" customWidth="1"/>
-    <col min="7" max="7" width="12.6328125" customWidth="1"/>
-    <col min="8" max="8" width="45.36328125" customWidth="1"/>
-    <col min="9" max="9" width="25.6328125" customWidth="1"/>
-    <col min="10" max="10" width="29.6328125" style="30" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.61328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.3828125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.84375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.61328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.61328125" customWidth="1"/>
+    <col min="6" max="6" width="45.3828125" customWidth="1"/>
+    <col min="7" max="7" width="12.61328125" customWidth="1"/>
+    <col min="8" max="8" width="45.3828125" customWidth="1"/>
+    <col min="9" max="9" width="25.61328125" customWidth="1"/>
+    <col min="10" max="10" width="29.61328125" style="30" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="32" style="30" customWidth="1"/>
-    <col min="12" max="12" width="31.36328125" style="30" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.81640625" style="30" customWidth="1"/>
-    <col min="14" max="14" width="26.6328125" style="30" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.36328125" style="30" customWidth="1"/>
-    <col min="16" max="16" width="23.6328125" customWidth="1"/>
-    <col min="17" max="17" width="31.1796875" customWidth="1"/>
+    <col min="12" max="12" width="31.3828125" style="30" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.84375" style="30" customWidth="1"/>
+    <col min="14" max="14" width="26.61328125" style="30" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.3828125" style="30" customWidth="1"/>
+    <col min="16" max="16" width="23.61328125" customWidth="1"/>
+    <col min="17" max="17" width="31.15234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -6819,7 +6837,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:17" ht="78" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="77.150000000000006" x14ac:dyDescent="0.35">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6" t="s">
@@ -6921,7 +6939,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11">
         <v>42736</v>
       </c>
@@ -6950,7 +6968,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>42736</v>
       </c>
@@ -6987,7 +7005,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>42736</v>
       </c>
@@ -7024,7 +7042,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>42736</v>
       </c>
@@ -7061,7 +7079,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>42736</v>
       </c>
@@ -7098,7 +7116,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>42736</v>
       </c>
@@ -7135,7 +7153,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>42736</v>
       </c>
@@ -7170,7 +7188,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <v>42736</v>
       </c>
@@ -7207,7 +7225,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>42736</v>
       </c>
@@ -7244,7 +7262,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>42736</v>
       </c>
@@ -7281,7 +7299,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="13">
         <v>42736</v>
       </c>
@@ -7318,7 +7336,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="13">
         <v>42736</v>
       </c>
@@ -7385,25 +7403,25 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.3828125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.3828125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.3828125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="20.6328125" customWidth="1"/>
-    <col min="6" max="7" width="20.6328125" style="14" customWidth="1"/>
-    <col min="8" max="8" width="21.6328125" customWidth="1"/>
-    <col min="9" max="9" width="21.6328125" style="14" customWidth="1"/>
-    <col min="10" max="10" width="14.36328125" customWidth="1"/>
-    <col min="11" max="11" width="12.81640625" customWidth="1"/>
-    <col min="12" max="12" width="15.81640625" customWidth="1"/>
-    <col min="13" max="13" width="28.6328125" customWidth="1"/>
-    <col min="14" max="14" width="28.6328125" style="14" customWidth="1"/>
-    <col min="15" max="15" width="23.36328125" customWidth="1"/>
+    <col min="5" max="5" width="20.61328125" customWidth="1"/>
+    <col min="6" max="7" width="20.61328125" style="14" customWidth="1"/>
+    <col min="8" max="8" width="21.61328125" customWidth="1"/>
+    <col min="9" max="9" width="21.61328125" style="14" customWidth="1"/>
+    <col min="10" max="10" width="14.3828125" customWidth="1"/>
+    <col min="11" max="11" width="12.84375" customWidth="1"/>
+    <col min="12" max="12" width="15.84375" customWidth="1"/>
+    <col min="13" max="13" width="28.61328125" customWidth="1"/>
+    <col min="14" max="14" width="28.61328125" style="14" customWidth="1"/>
+    <col min="15" max="15" width="23.3828125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>101</v>
       </c>
@@ -7424,7 +7442,7 @@
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
     </row>
-    <row r="2" spans="1:15" s="47" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="47" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="43"/>
       <c r="B2" s="43"/>
       <c r="C2" s="43" t="s">
@@ -7467,7 +7485,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="17.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -7514,7 +7532,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>42736</v>
       </c>
@@ -7551,7 +7569,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>42736</v>
       </c>
@@ -7588,7 +7606,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>42736</v>
       </c>
@@ -7625,7 +7643,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>42736</v>
       </c>
@@ -7662,7 +7680,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>42736</v>
       </c>
@@ -7699,7 +7717,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>42736</v>
       </c>
@@ -7736,7 +7754,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>42736</v>
       </c>
@@ -7773,7 +7791,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <v>42736</v>
       </c>
@@ -7810,7 +7828,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>42736</v>
       </c>
@@ -7847,7 +7865,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>42736</v>
       </c>
@@ -7884,7 +7902,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="13">
         <v>42736</v>
       </c>
@@ -7921,7 +7939,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="13">
         <v>42736</v>
       </c>
@@ -7958,7 +7976,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="13">
         <v>42736</v>
       </c>
@@ -7995,7 +8013,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13">
         <v>42736</v>
       </c>
@@ -8032,7 +8050,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="13">
         <v>42736</v>
       </c>
@@ -8069,7 +8087,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13">
         <v>42736</v>
       </c>
@@ -8106,7 +8124,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13">
         <v>42736</v>
       </c>
@@ -8143,7 +8161,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13">
         <v>42736</v>
       </c>
@@ -8180,7 +8198,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13">
         <v>42736</v>
       </c>
@@ -8217,7 +8235,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13">
         <v>42736</v>
       </c>
@@ -8254,7 +8272,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="13">
         <v>42736</v>
       </c>
@@ -8291,7 +8309,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="13">
         <v>42736</v>
       </c>
@@ -8328,7 +8346,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="13">
         <v>42736</v>
       </c>
@@ -8365,7 +8383,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="13">
         <v>42736</v>
       </c>
@@ -8402,7 +8420,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="13">
         <v>42736</v>
       </c>
@@ -8439,7 +8457,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="13">
         <v>42736</v>
       </c>
@@ -8476,7 +8494,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="13">
         <v>42736</v>
       </c>
@@ -8513,7 +8531,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="13">
         <v>42736</v>
       </c>
@@ -8550,7 +8568,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="13">
         <v>42736</v>
       </c>
@@ -8587,7 +8605,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="13">
         <v>42736</v>
       </c>
@@ -8624,7 +8642,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="13">
         <v>42736</v>
       </c>
@@ -8661,7 +8679,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="13">
         <v>42736</v>
       </c>
@@ -8698,7 +8716,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="13">
         <v>42736</v>
       </c>
@@ -8735,7 +8753,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="13">
         <v>42736</v>
       </c>
@@ -8772,7 +8790,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="13">
         <v>42736</v>
       </c>
@@ -8809,7 +8827,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="13">
         <v>42736</v>
       </c>
@@ -8846,7 +8864,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="13">
         <v>42736</v>
       </c>
@@ -8883,7 +8901,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="13">
         <v>42736</v>
       </c>
@@ -8920,7 +8938,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="13">
         <v>42736</v>
       </c>
@@ -8957,7 +8975,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="13">
         <v>42736</v>
       </c>
@@ -8994,7 +9012,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="13">
         <v>42736</v>
       </c>
@@ -9031,7 +9049,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="13">
         <v>42736</v>
       </c>
@@ -9068,7 +9086,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="13">
         <v>42736</v>
       </c>
@@ -9105,7 +9123,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="13">
         <v>42736</v>
       </c>
@@ -9142,7 +9160,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="13">
         <v>42736</v>
       </c>
@@ -9179,7 +9197,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="13">
         <v>42736</v>
       </c>
@@ -9216,7 +9234,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="50" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="13">
         <v>42736</v>
       </c>
@@ -9253,7 +9271,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="51" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="13">
         <v>42736</v>
       </c>
@@ -9290,7 +9308,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="52" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="13">
         <v>42736</v>
       </c>
@@ -9327,7 +9345,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="53" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="13">
         <v>42736</v>
       </c>
@@ -9364,7 +9382,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="54" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="13">
         <v>42736</v>
       </c>
@@ -9401,7 +9419,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="55" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="13">
         <v>42736</v>
       </c>
@@ -9438,7 +9456,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="56" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="13">
         <v>42736</v>
       </c>
@@ -9475,7 +9493,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="57" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="13">
         <v>42736</v>
       </c>
@@ -9512,7 +9530,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="58" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="13">
         <v>42736</v>
       </c>
@@ -9549,7 +9567,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="59" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="13">
         <v>42736</v>
       </c>
@@ -9586,7 +9604,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="60" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="13">
         <v>42736</v>
       </c>
@@ -9623,7 +9641,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="61" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="13">
         <v>42736</v>
       </c>
@@ -9660,7 +9678,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="62" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="13">
         <v>42736</v>
       </c>
@@ -9697,7 +9715,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="63" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="13">
         <v>42736</v>
       </c>
@@ -9734,7 +9752,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="64" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="13">
         <v>42736</v>
       </c>
@@ -9771,7 +9789,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="65" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="13">
         <v>42736</v>
       </c>
@@ -9808,7 +9826,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="66" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="13">
         <v>42736</v>
       </c>
@@ -9845,7 +9863,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="13">
         <v>42736</v>
       </c>
@@ -9882,7 +9900,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="13">
         <v>42736</v>
       </c>
@@ -9919,7 +9937,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="13">
         <v>42736</v>
       </c>
@@ -9956,7 +9974,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="13">
         <v>42736</v>
       </c>
@@ -9993,7 +10011,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="71" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="13">
         <v>42736</v>
       </c>
@@ -10030,7 +10048,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="13">
         <v>42736</v>
       </c>
@@ -10067,7 +10085,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="73" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="13">
         <v>42736</v>
       </c>
@@ -10104,7 +10122,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="13">
         <v>42736</v>
       </c>
@@ -10141,7 +10159,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="13">
         <v>42736</v>
       </c>
@@ -10178,7 +10196,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="76" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="13">
         <v>42736</v>
       </c>
@@ -10215,7 +10233,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="77" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="13">
         <v>42736</v>
       </c>
@@ -10252,7 +10270,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="13">
         <v>42736</v>
       </c>
@@ -10289,7 +10307,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="79" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="13">
         <v>42736</v>
       </c>
@@ -10326,7 +10344,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="80" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="13">
         <v>42736</v>
       </c>
@@ -10363,7 +10381,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="81" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="13">
         <v>42736</v>
       </c>
@@ -10400,7 +10418,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="82" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="13">
         <v>42736</v>
       </c>
@@ -10437,7 +10455,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="83" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="13">
         <v>42736</v>
       </c>
@@ -10474,7 +10492,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="84" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="13">
         <v>42736</v>
       </c>
@@ -10511,7 +10529,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="85" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="13">
         <v>42736</v>
       </c>
@@ -10548,7 +10566,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="86" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="13">
         <v>42736</v>
       </c>
@@ -10585,7 +10603,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="87" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="13">
         <v>42736</v>
       </c>
@@ -10622,7 +10640,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="88" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="13">
         <v>42736</v>
       </c>
@@ -10659,7 +10677,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="89" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="13">
         <v>42736</v>
       </c>
@@ -10696,7 +10714,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="90" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="13">
         <v>42736</v>
       </c>
@@ -10733,7 +10751,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="91" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="13">
         <v>42736</v>
       </c>
@@ -10797,17 +10815,17 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.3828125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.81640625" customWidth="1"/>
-    <col min="2" max="2" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.1796875" customWidth="1"/>
-    <col min="4" max="4" width="21.36328125" customWidth="1"/>
-    <col min="5" max="5" width="20.1796875" customWidth="1"/>
-    <col min="6" max="6" width="15.36328125" customWidth="1"/>
+    <col min="1" max="1" width="18.84375" customWidth="1"/>
+    <col min="2" max="2" width="15.3828125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.15234375" customWidth="1"/>
+    <col min="4" max="4" width="21.3828125" customWidth="1"/>
+    <col min="5" max="5" width="20.15234375" customWidth="1"/>
+    <col min="6" max="6" width="15.3828125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
@@ -10823,7 +10841,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" s="30" customFormat="1" ht="39" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="30" customFormat="1" ht="38.6" x14ac:dyDescent="0.35">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="31" t="s">
@@ -10839,7 +10857,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="14.6" x14ac:dyDescent="0.4">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -10859,7 +10877,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="14.6" x14ac:dyDescent="0.4">
       <c r="A4" s="11">
         <v>42736</v>
       </c>
@@ -10877,7 +10895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="14" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" s="14" customFormat="1" ht="14.6" x14ac:dyDescent="0.4">
       <c r="A5" s="13">
         <v>42736</v>
       </c>

</xml_diff>